<commit_message>
EE-1868 - Fixed EOL issues and improved error reports For further information, go to: https://www.ebi.ac.uk/panda/jira/browse/EE-1868?focusedCommentId=357329&page=com.atlassian.jira.plugin.system.issuetabpanels%3Acomment-tabpanel#comment-357329
</commit_message>
<xml_diff>
--- a/templates/sequence-based-metadata/EGA_metadata_submission_template_v1.xlsx
+++ b/templates/sequence-based-metadata/EGA_metadata_submission_template_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcasado\Documents\GitHub\ega-metadata-schema\templates\sequence-based-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5A1BE9-3E9C-4135-9C01-A7E32563A09B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736BA5D3-E7F2-43D4-8469-10048A091CAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2781,7 +2781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2877,7 +2877,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3105,18 +3104,6 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3148,13 +3135,25 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="111">
+  <dxfs count="93">
     <dxf>
       <fill>
         <patternFill>
@@ -4006,168 +4005,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFB7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFB7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFB7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4515,79 +4352,79 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="154" t="s">
         <v>401</v>
       </c>
-      <c r="B2" s="144"/>
+      <c r="B2" s="155"/>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="96" t="s">
         <v>402</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="96" t="s">
         <v>404</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="98" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="96" t="s">
         <v>406</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="98" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="96" t="s">
         <v>408</v>
       </c>
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="98" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="96" t="s">
         <v>410</v>
       </c>
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="98" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="96" t="s">
         <v>540</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="98" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="97" t="s">
         <v>412</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="98" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="145" t="s">
+      <c r="A10" s="156" t="s">
         <v>413</v>
       </c>
-      <c r="B10" s="145"/>
+      <c r="B10" s="156"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="146" t="s">
+      <c r="A12" s="157" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="144"/>
+      <c r="B12" s="155"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
@@ -4598,43 +4435,43 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="90">
+      <c r="A14" s="89">
         <v>1</v>
       </c>
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="98" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="91">
+      <c r="A15" s="90">
         <v>2</v>
       </c>
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="98" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="91">
+      <c r="A16" s="90">
         <v>3</v>
       </c>
-      <c r="B16" s="99" t="s">
+      <c r="B16" s="98" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="91" t="s">
+      <c r="A17" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="98" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="146" t="s">
+      <c r="A19" s="157" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="144"/>
+      <c r="B19" s="155"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
@@ -4645,42 +4482,42 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="92" t="s">
+      <c r="A21" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="100" t="s">
+      <c r="B21" s="99" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="93" t="s">
+      <c r="A22" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="99" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="99" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="95" t="s">
+      <c r="A24" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="99" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="96" t="s">
+      <c r="A25" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="100" t="s">
+      <c r="B25" s="99" t="s">
         <v>419</v>
       </c>
     </row>
@@ -4711,14 +4548,14 @@
     <col min="4" max="8" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" style="25" customWidth="1"/>
     <col min="10" max="11" width="8.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="88" customWidth="1"/>
-    <col min="13" max="14" width="8.7109375" style="151" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="88" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="87" customWidth="1"/>
+    <col min="13" max="14" width="8.7109375" style="146" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="87" customWidth="1"/>
     <col min="16" max="16" width="8.7109375" style="1" customWidth="1"/>
-    <col min="17" max="18" width="8.7109375" style="155" customWidth="1"/>
+    <col min="17" max="18" width="8.7109375" style="150" customWidth="1"/>
     <col min="19" max="19" width="8.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8" style="65" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" style="64" customWidth="1"/>
     <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8" customWidth="1"/>
   </cols>
@@ -4760,10 +4597,10 @@
       <c r="L1" s="23" t="s">
         <v>529</v>
       </c>
-      <c r="M1" s="148" t="s">
+      <c r="M1" s="143" t="s">
         <v>530</v>
       </c>
-      <c r="N1" s="148" t="s">
+      <c r="N1" s="143" t="s">
         <v>531</v>
       </c>
       <c r="O1" s="23" t="s">
@@ -4772,51 +4609,51 @@
       <c r="P1" s="23" t="s">
         <v>529</v>
       </c>
-      <c r="Q1" s="148" t="s">
+      <c r="Q1" s="143" t="s">
         <v>530</v>
       </c>
-      <c r="R1" s="148" t="s">
+      <c r="R1" s="143" t="s">
         <v>531</v>
       </c>
       <c r="S1" s="23" t="s">
         <v>532</v>
       </c>
-      <c r="T1" s="64" t="s">
+      <c r="T1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="V1" s="64" t="s">
+      <c r="V1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="W1" s="64" t="s">
+      <c r="W1" s="63" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="132" t="s">
         <v>548</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="133" t="s">
+      <c r="C2" s="132" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="133" t="s">
+      <c r="D2" s="132" t="s">
         <v>549</v>
       </c>
-      <c r="E2" s="133" t="s">
+      <c r="E2" s="132" t="s">
         <v>550</v>
       </c>
-      <c r="F2" s="157" t="s">
+      <c r="F2" s="152" t="s">
         <v>551</v>
       </c>
-      <c r="G2" s="133" t="s">
+      <c r="G2" s="132" t="s">
         <v>556</v>
       </c>
-      <c r="H2" s="133" t="s">
+      <c r="H2" s="132" t="s">
         <v>557</v>
       </c>
       <c r="I2" s="30" t="s">
@@ -4828,34 +4665,34 @@
       <c r="K2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="89" t="s">
+      <c r="L2" s="88" t="s">
         <v>552</v>
       </c>
-      <c r="M2" s="158" t="s">
+      <c r="M2" s="153" t="s">
         <v>553</v>
       </c>
-      <c r="N2" s="158" t="s">
+      <c r="N2" s="153" t="s">
         <v>554</v>
       </c>
-      <c r="O2" s="89" t="s">
+      <c r="O2" s="88" t="s">
         <v>555</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>552</v>
       </c>
-      <c r="Q2" s="153" t="s">
+      <c r="Q2" s="148" t="s">
         <v>553</v>
       </c>
-      <c r="R2" s="153" t="s">
+      <c r="R2" s="148" t="s">
         <v>554</v>
       </c>
       <c r="S2" s="15" t="s">
         <v>555</v>
       </c>
-      <c r="T2" s="66" t="s">
+      <c r="T2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="U2" s="66" t="s">
+      <c r="U2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="V2" s="29" t="s">
@@ -4869,11 +4706,11 @@
       <c r="A3" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="134"/>
-      <c r="M3" s="150"/>
-      <c r="N3" s="150"/>
-      <c r="Q3" s="150"/>
-      <c r="R3" s="150"/>
+      <c r="I3" s="133"/>
+      <c r="M3" s="145"/>
+      <c r="N3" s="145"/>
+      <c r="Q3" s="145"/>
+      <c r="R3" s="145"/>
     </row>
     <row r="4" spans="1:23" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
@@ -4894,7 +4731,7 @@
       <c r="F4" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="H4" s="156" t="s">
+      <c r="H4" s="151" t="s">
         <v>543</v>
       </c>
       <c r="I4" s="30" t="s">
@@ -4904,40 +4741,40 @@
         <v>441</v>
       </c>
       <c r="K4" s="31"/>
-      <c r="L4" s="147" t="s">
+      <c r="L4" s="142" t="s">
         <v>533</v>
       </c>
-      <c r="M4" s="149" t="s">
+      <c r="M4" s="144" t="s">
         <v>534</v>
       </c>
-      <c r="N4" s="149" t="s">
+      <c r="N4" s="144" t="s">
         <v>535</v>
       </c>
-      <c r="O4" s="152" t="s">
+      <c r="O4" s="147" t="s">
         <v>539</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>533</v>
       </c>
-      <c r="Q4" s="153" t="s">
+      <c r="Q4" s="148" t="s">
         <v>536</v>
       </c>
-      <c r="R4" s="153" t="s">
+      <c r="R4" s="148" t="s">
         <v>537</v>
       </c>
-      <c r="S4" s="154" t="s">
+      <c r="S4" s="149" t="s">
         <v>538</v>
       </c>
-      <c r="T4" s="109" t="s">
+      <c r="T4" s="108" t="s">
         <v>517</v>
       </c>
-      <c r="U4" s="140" t="s">
+      <c r="U4" s="139" t="s">
         <v>518</v>
       </c>
       <c r="V4" s="44" t="s">
         <v>519</v>
       </c>
-      <c r="W4" s="111" t="s">
+      <c r="W4" s="110" t="s">
         <v>444</v>
       </c>
     </row>
@@ -5006,19 +4843,19 @@
     <col min="16" max="18" width="8.7109375" style="2" customWidth="1"/>
     <col min="19" max="22" width="10.85546875" style="35" customWidth="1"/>
     <col min="23" max="26" width="10.85546875" customWidth="1"/>
-    <col min="27" max="27" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" style="65" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" style="64" customWidth="1"/>
     <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="87" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" style="63" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13" style="63" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" style="62" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13" style="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
@@ -5100,43 +4937,43 @@
       <c r="Z1" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" s="64" t="s">
+      <c r="AA1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="AB1" s="64" t="s">
+      <c r="AB1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="AC1" s="64" t="s">
+      <c r="AC1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="AD1" s="64" t="s">
+      <c r="AD1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="AE1" s="87" t="s">
+      <c r="AE1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="AF1" s="87" t="s">
+      <c r="AF1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="AG1" s="87" t="s">
+      <c r="AG1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="AH1" s="87" t="s">
+      <c r="AH1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="AI1" s="87" t="s">
+      <c r="AI1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="AJ1" s="87" t="s">
+      <c r="AJ1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="AK1" s="61" t="s">
+      <c r="AK1" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="AL1" s="61" t="s">
+      <c r="AL1" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="AM1" s="61" t="s">
+      <c r="AM1" s="60" t="s">
         <v>359</v>
       </c>
     </row>
@@ -5195,16 +5032,16 @@
       <c r="R2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="78" t="s">
+      <c r="S2" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="T2" s="78" t="s">
+      <c r="T2" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="U2" s="78" t="s">
+      <c r="U2" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="V2" s="78" t="s">
+      <c r="V2" s="77" t="s">
         <v>151</v>
       </c>
       <c r="W2" s="24" t="s">
@@ -5219,10 +5056,10 @@
       <c r="Z2" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="AA2" s="66" t="s">
+      <c r="AA2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="AB2" s="66" t="s">
+      <c r="AB2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="AC2" s="29" t="s">
@@ -5231,13 +5068,13 @@
       <c r="AD2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="AE2" s="89" t="s">
+      <c r="AE2" s="88" t="s">
         <v>474</v>
       </c>
-      <c r="AF2" s="89" t="s">
+      <c r="AF2" s="88" t="s">
         <v>475</v>
       </c>
-      <c r="AG2" s="89" t="s">
+      <c r="AG2" s="88" t="s">
         <v>362</v>
       </c>
       <c r="AH2" s="24" t="s">
@@ -5249,13 +5086,13 @@
       <c r="AJ2" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="AK2" s="62" t="s">
+      <c r="AK2" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="AL2" s="62" t="s">
+      <c r="AL2" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="AM2" s="62" t="s">
+      <c r="AM2" s="61" t="s">
         <v>364</v>
       </c>
     </row>
@@ -5334,10 +5171,10 @@
       <c r="Z4" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="AA4" s="65" t="s">
+      <c r="AA4" s="64" t="s">
         <v>365</v>
       </c>
-      <c r="AB4" s="65" t="s">
+      <c r="AB4" s="64" t="s">
         <v>366</v>
       </c>
       <c r="AC4" t="s">
@@ -5346,13 +5183,13 @@
       <c r="AD4" t="s">
         <v>368</v>
       </c>
-      <c r="AE4" s="88" t="s">
+      <c r="AE4" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="AF4" s="88" t="s">
+      <c r="AF4" s="87" t="s">
         <v>469</v>
       </c>
-      <c r="AG4" s="88" t="s">
+      <c r="AG4" s="87" t="s">
         <v>472</v>
       </c>
       <c r="AH4" t="s">
@@ -5364,13 +5201,13 @@
       <c r="AJ4" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="AK4" s="63" t="s">
+      <c r="AK4" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="AL4" s="63">
+      <c r="AL4" s="62">
         <v>289</v>
       </c>
-      <c r="AM4" s="63" t="s">
+      <c r="AM4" s="62" t="s">
         <v>370</v>
       </c>
     </row>
@@ -5476,19 +5313,19 @@
     <col min="24" max="24" width="6.42578125" style="2" customWidth="1"/>
     <col min="25" max="25" width="6.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.28515625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" style="65" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" style="64" customWidth="1"/>
     <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="87" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" style="63" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13" style="63" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" style="62" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13" style="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
@@ -5516,31 +5353,31 @@
       <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="49" t="s">
+      <c r="Q1" s="48" t="s">
         <v>2</v>
       </c>
       <c r="R1" s="22" t="s">
@@ -5570,43 +5407,43 @@
       <c r="Z1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="64" t="s">
+      <c r="AA1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="AB1" s="64" t="s">
+      <c r="AB1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="AC1" s="64" t="s">
+      <c r="AC1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="AD1" s="64" t="s">
+      <c r="AD1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="AE1" s="87" t="s">
+      <c r="AE1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="AF1" s="87" t="s">
+      <c r="AF1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="AG1" s="87" t="s">
+      <c r="AG1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="AH1" s="87" t="s">
+      <c r="AH1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="AI1" s="87" t="s">
+      <c r="AI1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="AJ1" s="87" t="s">
+      <c r="AJ1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="AK1" s="61" t="s">
+      <c r="AK1" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="AL1" s="61" t="s">
+      <c r="AL1" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="AM1" s="61" t="s">
+      <c r="AM1" s="60" t="s">
         <v>359</v>
       </c>
     </row>
@@ -5645,7 +5482,7 @@
       <c r="L2" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="M2" s="54" t="s">
+      <c r="M2" s="53" t="s">
         <v>295</v>
       </c>
       <c r="N2" s="31"/>
@@ -5683,10 +5520,10 @@
       <c r="Z2" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="AA2" s="66" t="s">
+      <c r="AA2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="AB2" s="66" t="s">
+      <c r="AB2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="AC2" s="29" t="s">
@@ -5695,13 +5532,13 @@
       <c r="AD2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="AE2" s="89" t="s">
+      <c r="AE2" s="88" t="s">
         <v>474</v>
       </c>
-      <c r="AF2" s="89" t="s">
+      <c r="AF2" s="88" t="s">
         <v>475</v>
       </c>
-      <c r="AG2" s="89" t="s">
+      <c r="AG2" s="88" t="s">
         <v>362</v>
       </c>
       <c r="AH2" s="24" t="s">
@@ -5713,13 +5550,13 @@
       <c r="AJ2" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="AK2" s="62" t="s">
+      <c r="AK2" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="AL2" s="62" t="s">
+      <c r="AL2" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="AM2" s="62" t="s">
+      <c r="AM2" s="61" t="s">
         <v>364</v>
       </c>
     </row>
@@ -5728,7 +5565,7 @@
         <v>103</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="R3" s="55"/>
+      <c r="R3" s="54"/>
       <c r="AA3" s="27"/>
       <c r="AB3" s="27"/>
       <c r="AC3" s="27"/>
@@ -5810,10 +5647,10 @@
       <c r="Y4" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="AA4" s="65" t="s">
+      <c r="AA4" s="64" t="s">
         <v>365</v>
       </c>
-      <c r="AB4" s="65" t="s">
+      <c r="AB4" s="64" t="s">
         <v>366</v>
       </c>
       <c r="AC4" t="s">
@@ -5822,13 +5659,13 @@
       <c r="AD4" t="s">
         <v>368</v>
       </c>
-      <c r="AE4" s="88" t="s">
+      <c r="AE4" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="AF4" s="88" t="s">
+      <c r="AF4" s="87" t="s">
         <v>469</v>
       </c>
-      <c r="AG4" s="88" t="s">
+      <c r="AG4" s="87" t="s">
         <v>472</v>
       </c>
       <c r="AH4" t="s">
@@ -5840,13 +5677,13 @@
       <c r="AJ4" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="AK4" s="63" t="s">
+      <c r="AK4" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="AL4" s="63">
+      <c r="AL4" s="62">
         <v>289</v>
       </c>
-      <c r="AM4" s="63" t="s">
+      <c r="AM4" s="62" t="s">
         <v>370</v>
       </c>
     </row>
@@ -5892,7 +5729,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B3225A-CA96-4372-AB7E-97999D11252D}">
-  <dimension ref="A1:BV16"/>
+  <dimension ref="A1:BV4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5915,25 +5752,25 @@
     <col min="37" max="38" width="15.5703125" style="46" customWidth="1"/>
     <col min="39" max="44" width="8.7109375" style="41" customWidth="1"/>
     <col min="45" max="50" width="8.7109375" customWidth="1"/>
-    <col min="51" max="51" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8" style="65" customWidth="1"/>
+    <col min="51" max="51" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8" style="64" customWidth="1"/>
     <col min="53" max="53" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="8" customWidth="1"/>
-    <col min="55" max="55" width="8.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.7109375" style="87" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11" style="63" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13" style="63" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11" style="62" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13" style="62" bestFit="1" customWidth="1"/>
     <col min="64" max="65" width="8.7109375" style="42" customWidth="1"/>
     <col min="66" max="67" width="8.7109375" customWidth="1"/>
     <col min="68" max="69" width="8.7109375" style="42" customWidth="1"/>
-    <col min="70" max="71" width="8.7109375" style="68" customWidth="1"/>
-    <col min="72" max="73" width="8.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.7109375" style="69" customWidth="1"/>
+    <col min="70" max="71" width="8.7109375" style="67" customWidth="1"/>
+    <col min="72" max="73" width="8.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.7109375" style="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6087,43 +5924,43 @@
       <c r="AX1" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="AY1" s="64" t="s">
+      <c r="AY1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="AZ1" s="64" t="s">
+      <c r="AZ1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="BA1" s="64" t="s">
+      <c r="BA1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="BB1" s="64" t="s">
+      <c r="BB1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="BC1" s="87" t="s">
+      <c r="BC1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="BD1" s="87" t="s">
+      <c r="BD1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="BE1" s="87" t="s">
+      <c r="BE1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="BF1" s="87" t="s">
+      <c r="BF1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="BG1" s="87" t="s">
+      <c r="BG1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="BH1" s="87" t="s">
+      <c r="BH1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="BI1" s="61" t="s">
+      <c r="BI1" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="BJ1" s="61" t="s">
+      <c r="BJ1" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="BK1" s="61" t="s">
+      <c r="BK1" s="60" t="s">
         <v>359</v>
       </c>
       <c r="BL1" s="39" t="s">
@@ -6150,13 +5987,13 @@
       <c r="BS1" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="BT1" s="87" t="s">
+      <c r="BT1" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="BU1" s="87" t="s">
+      <c r="BU1" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="BV1" s="67" t="s">
+      <c r="BV1" s="66" t="s">
         <v>208</v>
       </c>
     </row>
@@ -6182,7 +6019,7 @@
       <c r="G2" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="34" t="s">
         <v>214</v>
       </c>
       <c r="I2" s="24" t="s">
@@ -6257,10 +6094,10 @@
       <c r="AF2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="AG2" s="72" t="s">
+      <c r="AG2" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="AH2" s="72" t="s">
+      <c r="AH2" s="71" t="s">
         <v>220</v>
       </c>
       <c r="AI2" s="24" t="s">
@@ -6269,28 +6106,28 @@
       <c r="AJ2" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="AK2" s="72" t="s">
+      <c r="AK2" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="AL2" s="72" t="s">
+      <c r="AL2" s="71" t="s">
         <v>220</v>
       </c>
-      <c r="AM2" s="73" t="s">
+      <c r="AM2" s="72" t="s">
         <v>221</v>
       </c>
-      <c r="AN2" s="74" t="s">
+      <c r="AN2" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="AO2" s="73" t="s">
+      <c r="AO2" s="72" t="s">
         <v>223</v>
       </c>
-      <c r="AP2" s="73" t="s">
+      <c r="AP2" s="72" t="s">
         <v>224</v>
       </c>
-      <c r="AQ2" s="73" t="s">
+      <c r="AQ2" s="72" t="s">
         <v>225</v>
       </c>
-      <c r="AR2" s="73" t="s">
+      <c r="AR2" s="72" t="s">
         <v>226</v>
       </c>
       <c r="AS2" s="29" t="s">
@@ -6311,10 +6148,10 @@
       <c r="AX2" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="AY2" s="66" t="s">
+      <c r="AY2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="AZ2" s="66" t="s">
+      <c r="AZ2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="BA2" s="29" t="s">
@@ -6323,13 +6160,13 @@
       <c r="BB2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="BC2" s="89" t="s">
+      <c r="BC2" s="88" t="s">
         <v>474</v>
       </c>
-      <c r="BD2" s="89" t="s">
+      <c r="BD2" s="88" t="s">
         <v>475</v>
       </c>
-      <c r="BE2" s="89" t="s">
+      <c r="BE2" s="88" t="s">
         <v>362</v>
       </c>
       <c r="BF2" s="24" t="s">
@@ -6341,19 +6178,19 @@
       <c r="BH2" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="BI2" s="62" t="s">
+      <c r="BI2" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="BJ2" s="62" t="s">
+      <c r="BJ2" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="BK2" s="62" t="s">
+      <c r="BK2" s="61" t="s">
         <v>364</v>
       </c>
-      <c r="BL2" s="75" t="s">
+      <c r="BL2" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="BM2" s="75" t="s">
+      <c r="BM2" s="74" t="s">
         <v>229</v>
       </c>
       <c r="BN2" s="29" t="s">
@@ -6362,25 +6199,25 @@
       <c r="BO2" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="BP2" s="75" t="s">
+      <c r="BP2" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="BQ2" s="75" t="s">
+      <c r="BQ2" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="BR2" s="76" t="s">
+      <c r="BR2" s="75" t="s">
         <v>230</v>
       </c>
-      <c r="BS2" s="76" t="s">
+      <c r="BS2" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="BT2" s="89" t="s">
+      <c r="BT2" s="88" t="s">
         <v>232</v>
       </c>
-      <c r="BU2" s="89" t="s">
+      <c r="BU2" s="88" t="s">
         <v>233</v>
       </c>
-      <c r="BV2" s="77" t="s">
+      <c r="BV2" s="76" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6389,7 +6226,7 @@
         <v>103</v>
       </c>
       <c r="L3" s="18"/>
-      <c r="AD3" s="55"/>
+      <c r="AD3" s="54"/>
       <c r="AY3" s="27"/>
       <c r="AZ3" s="27"/>
       <c r="BA3" s="27"/>
@@ -6431,7 +6268,7 @@
       <c r="H4" t="s">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="43" t="s">
         <v>239</v>
       </c>
       <c r="J4" t="s">
@@ -6548,10 +6385,10 @@
       <c r="AW4" t="s">
         <v>272</v>
       </c>
-      <c r="AY4" s="65" t="s">
+      <c r="AY4" s="64" t="s">
         <v>365</v>
       </c>
-      <c r="AZ4" s="65" t="s">
+      <c r="AZ4" s="64" t="s">
         <v>366</v>
       </c>
       <c r="BA4" t="s">
@@ -6560,13 +6397,13 @@
       <c r="BB4" t="s">
         <v>368</v>
       </c>
-      <c r="BC4" s="88" t="s">
+      <c r="BC4" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="BD4" s="88" t="s">
+      <c r="BD4" s="87" t="s">
         <v>469</v>
       </c>
-      <c r="BE4" s="88" t="s">
+      <c r="BE4" s="87" t="s">
         <v>472</v>
       </c>
       <c r="BF4" t="s">
@@ -6578,13 +6415,13 @@
       <c r="BH4" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="BI4" s="63" t="s">
+      <c r="BI4" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="BJ4" s="63">
+      <c r="BJ4" s="62">
         <v>289</v>
       </c>
-      <c r="BK4" s="63" t="s">
+      <c r="BK4" s="62" t="s">
         <v>370</v>
       </c>
       <c r="BL4" s="42" t="s">
@@ -6599,21 +6436,18 @@
       <c r="BP4" s="42" t="s">
         <v>276</v>
       </c>
-      <c r="BR4" s="68" t="s">
+      <c r="BR4" s="67" t="s">
         <v>277</v>
       </c>
-      <c r="BT4" s="88" t="s">
+      <c r="BT4" s="87" t="s">
         <v>278</v>
       </c>
-      <c r="BU4" s="88" t="s">
+      <c r="BU4" s="87" t="s">
         <v>279</v>
       </c>
-      <c r="BV4" s="69" t="s">
+      <c r="BV4" s="68" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="16" spans="1:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="47"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1 AE1:AF1 AM1:AR1 BV1:XFD1 BL1:BM1 H1:I1 M1:AC1">
@@ -6733,25 +6567,25 @@
     <col min="14" max="14" width="15.5703125" style="7" customWidth="1"/>
     <col min="15" max="18" width="15.5703125" style="8" customWidth="1"/>
     <col min="19" max="30" width="15.5703125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="71" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" style="70" customWidth="1"/>
     <col min="32" max="41" width="8.7109375" style="11" customWidth="1"/>
     <col min="42" max="46" width="8.7109375" style="13" customWidth="1"/>
     <col min="47" max="51" width="8.7109375" style="9" customWidth="1"/>
     <col min="52" max="54" width="8.7109375" style="3" customWidth="1"/>
     <col min="55" max="55" width="9.140625" style="10"/>
-    <col min="58" max="58" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8" style="65" customWidth="1"/>
+    <col min="58" max="58" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8" style="64" customWidth="1"/>
     <col min="60" max="60" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="8" customWidth="1"/>
-    <col min="62" max="62" width="8.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.7109375" style="87" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11" style="63" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13" style="63" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11" style="62" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="10.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13" style="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.25">
@@ -6845,7 +6679,7 @@
       <c r="AD1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AE1" s="70" t="s">
+      <c r="AE1" s="69" t="s">
         <v>389</v>
       </c>
       <c r="AF1" s="12" t="s">
@@ -6926,43 +6760,43 @@
       <c r="BE1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="BF1" s="64" t="s">
+      <c r="BF1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="BG1" s="64" t="s">
+      <c r="BG1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="BH1" s="64" t="s">
+      <c r="BH1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="BI1" s="64" t="s">
+      <c r="BI1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="BJ1" s="87" t="s">
+      <c r="BJ1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="BK1" s="87" t="s">
+      <c r="BK1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="BL1" s="87" t="s">
+      <c r="BL1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="BM1" s="87" t="s">
+      <c r="BM1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="BN1" s="87" t="s">
+      <c r="BN1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="BO1" s="87" t="s">
+      <c r="BO1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="BP1" s="61" t="s">
+      <c r="BP1" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="BQ1" s="61" t="s">
+      <c r="BQ1" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="BR1" s="61" t="s">
+      <c r="BR1" s="60" t="s">
         <v>359</v>
       </c>
     </row>
@@ -7006,7 +6840,7 @@
       <c r="M2" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="N2" s="79" t="s">
+      <c r="N2" s="78" t="s">
         <v>122</v>
       </c>
       <c r="O2" s="15" t="s">
@@ -7057,91 +6891,91 @@
       <c r="AD2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="AE2" s="80" t="s">
+      <c r="AE2" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="AF2" s="81" t="s">
+      <c r="AF2" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="AG2" s="81" t="s">
+      <c r="AG2" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="AH2" s="81" t="s">
+      <c r="AH2" s="80" t="s">
         <v>400</v>
       </c>
-      <c r="AI2" s="81" t="s">
+      <c r="AI2" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="AJ2" s="81" t="s">
+      <c r="AJ2" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="AK2" s="81" t="s">
+      <c r="AK2" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="AL2" s="81" t="s">
+      <c r="AL2" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="AM2" s="81" t="s">
+      <c r="AM2" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="AN2" s="81" t="s">
+      <c r="AN2" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="AO2" s="81" t="s">
+      <c r="AO2" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="AP2" s="82" t="s">
+      <c r="AP2" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="AQ2" s="82" t="s">
+      <c r="AQ2" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="AR2" s="82" t="s">
+      <c r="AR2" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="AS2" s="82" t="s">
+      <c r="AS2" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="AT2" s="82" t="s">
+      <c r="AT2" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="AU2" s="83" t="s">
+      <c r="AU2" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="AV2" s="83" t="s">
+      <c r="AV2" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="AW2" s="83" t="s">
+      <c r="AW2" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="AX2" s="83" t="s">
+      <c r="AX2" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="AY2" s="83" t="s">
+      <c r="AY2" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="AZ2" s="84" t="s">
+      <c r="AZ2" s="83" t="s">
         <v>5</v>
       </c>
       <c r="BA2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="BB2" s="84" t="s">
+      <c r="BB2" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="BC2" s="83" t="s">
+      <c r="BC2" s="82" t="s">
         <v>5</v>
       </c>
       <c r="BD2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="BE2" s="83" t="s">
+      <c r="BE2" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="BF2" s="66" t="s">
+      <c r="BF2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="BG2" s="66" t="s">
+      <c r="BG2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="BH2" s="29" t="s">
@@ -7150,13 +6984,13 @@
       <c r="BI2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="BJ2" s="89" t="s">
+      <c r="BJ2" s="88" t="s">
         <v>474</v>
       </c>
-      <c r="BK2" s="89" t="s">
+      <c r="BK2" s="88" t="s">
         <v>475</v>
       </c>
-      <c r="BL2" s="89" t="s">
+      <c r="BL2" s="88" t="s">
         <v>362</v>
       </c>
       <c r="BM2" s="24" t="s">
@@ -7168,13 +7002,13 @@
       <c r="BO2" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="BP2" s="62" t="s">
+      <c r="BP2" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="BQ2" s="62" t="s">
+      <c r="BQ2" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="BR2" s="62" t="s">
+      <c r="BR2" s="61" t="s">
         <v>364</v>
       </c>
     </row>
@@ -7186,7 +7020,7 @@
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
       <c r="R3" s="21"/>
-      <c r="AE3" s="55"/>
+      <c r="AE3" s="54"/>
       <c r="BF3" s="27"/>
       <c r="BG3" s="27"/>
       <c r="BH3" s="27"/>
@@ -7301,10 +7135,10 @@
       <c r="BD4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="BF4" s="65" t="s">
+      <c r="BF4" s="64" t="s">
         <v>365</v>
       </c>
-      <c r="BG4" s="65" t="s">
+      <c r="BG4" s="64" t="s">
         <v>366</v>
       </c>
       <c r="BH4" t="s">
@@ -7313,13 +7147,13 @@
       <c r="BI4" t="s">
         <v>368</v>
       </c>
-      <c r="BJ4" s="88" t="s">
+      <c r="BJ4" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="BK4" s="88" t="s">
+      <c r="BK4" s="87" t="s">
         <v>469</v>
       </c>
-      <c r="BL4" s="88" t="s">
+      <c r="BL4" s="87" t="s">
         <v>472</v>
       </c>
       <c r="BM4" t="s">
@@ -7331,13 +7165,13 @@
       <c r="BO4" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="BP4" s="63" t="s">
+      <c r="BP4" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="BQ4" s="63">
+      <c r="BQ4" s="62">
         <v>289</v>
       </c>
-      <c r="BR4" s="63" t="s">
+      <c r="BR4" s="62" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7445,22 +7279,22 @@
     <col min="16" max="17" width="15.5703125" style="46" customWidth="1"/>
     <col min="18" max="19" width="15.5703125" customWidth="1"/>
     <col min="20" max="21" width="15.5703125" style="46" customWidth="1"/>
-    <col min="22" max="28" width="8.7109375" style="56" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="56"/>
+    <col min="22" max="28" width="8.7109375" style="55" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="55"/>
     <col min="30" max="36" width="8.7109375" customWidth="1"/>
-    <col min="38" max="38" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8" style="65" customWidth="1"/>
+    <col min="38" max="38" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" style="64" customWidth="1"/>
     <col min="40" max="40" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="8" customWidth="1"/>
-    <col min="42" max="42" width="8.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.7109375" style="87" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11" style="63" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13" style="63" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11" style="62" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13" style="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7482,7 +7316,7 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="59" t="s">
         <v>318</v>
       </c>
       <c r="H1" s="36" t="s">
@@ -7575,43 +7409,43 @@
       <c r="AK1" s="38" t="s">
         <v>321</v>
       </c>
-      <c r="AL1" s="64" t="s">
+      <c r="AL1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="AM1" s="64" t="s">
+      <c r="AM1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="AN1" s="64" t="s">
+      <c r="AN1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="AO1" s="64" t="s">
+      <c r="AO1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="AP1" s="87" t="s">
+      <c r="AP1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="AQ1" s="87" t="s">
+      <c r="AQ1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="AR1" s="87" t="s">
+      <c r="AR1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="AS1" s="87" t="s">
+      <c r="AS1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="AT1" s="87" t="s">
+      <c r="AT1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="AU1" s="87" t="s">
+      <c r="AU1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="AV1" s="61" t="s">
+      <c r="AV1" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="AW1" s="61" t="s">
+      <c r="AW1" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="AX1" s="61" t="s">
+      <c r="AX1" s="60" t="s">
         <v>359</v>
       </c>
     </row>
@@ -7661,10 +7495,10 @@
       <c r="O2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="P2" s="71" t="s">
         <v>328</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="Q2" s="71" t="s">
         <v>329</v>
       </c>
       <c r="R2" s="24" t="s">
@@ -7673,34 +7507,34 @@
       <c r="S2" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="T2" s="72" t="s">
+      <c r="T2" s="71" t="s">
         <v>328</v>
       </c>
-      <c r="U2" s="72" t="s">
+      <c r="U2" s="71" t="s">
         <v>329</v>
       </c>
-      <c r="V2" s="85" t="s">
+      <c r="V2" s="84" t="s">
         <v>330</v>
       </c>
-      <c r="W2" s="85" t="s">
+      <c r="W2" s="84" t="s">
         <v>331</v>
       </c>
-      <c r="X2" s="86" t="s">
+      <c r="X2" s="85" t="s">
         <v>223</v>
       </c>
-      <c r="Y2" s="86" t="s">
+      <c r="Y2" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="Z2" s="86" t="s">
+      <c r="Z2" s="85" t="s">
         <v>225</v>
       </c>
-      <c r="AA2" s="86" t="s">
+      <c r="AA2" s="85" t="s">
         <v>332</v>
       </c>
-      <c r="AB2" s="86" t="s">
+      <c r="AB2" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="AC2" s="86" t="s">
+      <c r="AC2" s="85" t="s">
         <v>334</v>
       </c>
       <c r="AD2" s="24" t="s">
@@ -7727,10 +7561,10 @@
       <c r="AK2" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="AL2" s="66" t="s">
+      <c r="AL2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="AM2" s="66" t="s">
+      <c r="AM2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="AN2" s="29" t="s">
@@ -7739,13 +7573,13 @@
       <c r="AO2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="AP2" s="89" t="s">
+      <c r="AP2" s="88" t="s">
         <v>474</v>
       </c>
-      <c r="AQ2" s="89" t="s">
+      <c r="AQ2" s="88" t="s">
         <v>475</v>
       </c>
-      <c r="AR2" s="89" t="s">
+      <c r="AR2" s="88" t="s">
         <v>362</v>
       </c>
       <c r="AS2" s="24" t="s">
@@ -7757,21 +7591,21 @@
       <c r="AU2" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="AV2" s="62" t="s">
+      <c r="AV2" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="AW2" s="62" t="s">
+      <c r="AW2" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="AX2" s="62" t="s">
+      <c r="AX2" s="61" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="58" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+    <row r="3" spans="1:50" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="M3" s="59"/>
+      <c r="M3" s="58"/>
       <c r="AL3" s="27"/>
       <c r="AM3" s="27"/>
       <c r="AN3" s="27"/>
@@ -7844,28 +7678,28 @@
       <c r="U4" s="46" t="s">
         <v>264</v>
       </c>
-      <c r="V4" s="56" t="s">
+      <c r="V4" s="55" t="s">
         <v>344</v>
       </c>
-      <c r="W4" s="56" t="s">
+      <c r="W4" s="55" t="s">
         <v>266</v>
       </c>
-      <c r="X4" s="56" t="s">
+      <c r="X4" s="55" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="56" t="s">
+      <c r="Y4" s="55" t="s">
         <v>271</v>
       </c>
-      <c r="Z4" s="56" t="s">
+      <c r="Z4" s="55" t="s">
         <v>272</v>
       </c>
-      <c r="AA4" s="56" t="s">
+      <c r="AA4" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="AB4" s="56" t="s">
+      <c r="AB4" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="AC4" s="56" t="s">
+      <c r="AC4" s="55" t="s">
         <v>347</v>
       </c>
       <c r="AD4" t="s">
@@ -7892,10 +7726,10 @@
       <c r="AK4" t="s">
         <v>347</v>
       </c>
-      <c r="AL4" s="65" t="s">
+      <c r="AL4" s="64" t="s">
         <v>365</v>
       </c>
-      <c r="AM4" s="65" t="s">
+      <c r="AM4" s="64" t="s">
         <v>366</v>
       </c>
       <c r="AN4" t="s">
@@ -7904,13 +7738,13 @@
       <c r="AO4" t="s">
         <v>368</v>
       </c>
-      <c r="AP4" s="88" t="s">
+      <c r="AP4" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="AQ4" s="88" t="s">
+      <c r="AQ4" s="87" t="s">
         <v>469</v>
       </c>
-      <c r="AR4" s="88" t="s">
+      <c r="AR4" s="87" t="s">
         <v>472</v>
       </c>
       <c r="AS4" t="s">
@@ -7922,13 +7756,13 @@
       <c r="AU4" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="AV4" s="63" t="s">
+      <c r="AV4" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="AW4" s="63">
+      <c r="AW4" s="62">
         <v>289</v>
       </c>
-      <c r="AX4" s="63" t="s">
+      <c r="AX4" s="62" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8006,31 +7840,31 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="104" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="103" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="107" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="106" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" style="3" customWidth="1"/>
     <col min="11" max="12" width="8.7109375" style="2" customWidth="1"/>
     <col min="13" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" style="65" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" style="64" customWidth="1"/>
     <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="87" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" style="63" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13" style="63" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="62" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13" style="62" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.42578125" style="116" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="115" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.42578125" style="116" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.42578125" style="115" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8053,13 +7887,13 @@
       <c r="F1" t="s">
         <v>424</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="101" t="s">
         <v>422</v>
       </c>
-      <c r="H1" s="105" t="s">
+      <c r="H1" s="104" t="s">
         <v>422</v>
       </c>
-      <c r="I1" s="105" t="s">
+      <c r="I1" s="104" t="s">
         <v>422</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -8080,61 +7914,61 @@
       <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="P1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="Q1" s="64" t="s">
+      <c r="Q1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="R1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="T1" s="87" t="s">
+      <c r="T1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="U1" s="87" t="s">
+      <c r="U1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="V1" s="87" t="s">
+      <c r="V1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="W1" s="87" t="s">
+      <c r="W1" s="86" t="s">
         <v>354</v>
       </c>
-      <c r="X1" s="87" t="s">
+      <c r="X1" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="Y1" s="87" t="s">
+      <c r="Y1" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="Z1" s="61" t="s">
+      <c r="Z1" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="AA1" s="61" t="s">
+      <c r="AA1" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="AB1" s="61" t="s">
+      <c r="AB1" s="60" t="s">
         <v>359</v>
       </c>
-      <c r="AC1" s="64" t="s">
+      <c r="AC1" s="63" t="s">
         <v>429</v>
       </c>
-      <c r="AD1" s="64" t="s">
+      <c r="AD1" s="63" t="s">
         <v>429</v>
       </c>
-      <c r="AE1" s="64" t="s">
+      <c r="AE1" s="63" t="s">
         <v>429</v>
       </c>
-      <c r="AF1" s="114" t="s">
+      <c r="AF1" s="113" t="s">
         <v>430</v>
       </c>
-      <c r="AG1" s="114" t="s">
+      <c r="AG1" s="113" t="s">
         <v>430</v>
       </c>
-      <c r="AH1" s="114" t="s">
+      <c r="AH1" s="113" t="s">
         <v>430</v>
       </c>
     </row>
@@ -8157,16 +7991,16 @@
       <c r="F2" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="G2" s="103" t="s">
+      <c r="G2" s="102" t="s">
         <v>433</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="H2" s="82" t="s">
         <v>433</v>
       </c>
-      <c r="I2" s="113" t="s">
+      <c r="I2" s="112" t="s">
         <v>433</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="83" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="31" t="s">
@@ -8184,10 +8018,10 @@
       <c r="O2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="66" t="s">
+      <c r="P2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="Q2" s="66" t="s">
+      <c r="Q2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="R2" s="29" t="s">
@@ -8196,13 +8030,13 @@
       <c r="S2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="T2" s="89" t="s">
+      <c r="T2" s="88" t="s">
         <v>474</v>
       </c>
-      <c r="U2" s="89" t="s">
+      <c r="U2" s="88" t="s">
         <v>475</v>
       </c>
-      <c r="V2" s="89" t="s">
+      <c r="V2" s="88" t="s">
         <v>362</v>
       </c>
       <c r="W2" s="24" t="s">
@@ -8214,31 +8048,31 @@
       <c r="Y2" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="Z2" s="62" t="s">
+      <c r="Z2" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="AA2" s="62" t="s">
+      <c r="AA2" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="AB2" s="62" t="s">
+      <c r="AB2" s="61" t="s">
         <v>364</v>
       </c>
-      <c r="AC2" s="66" t="s">
+      <c r="AC2" s="65" t="s">
         <v>447</v>
       </c>
       <c r="AD2" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="AE2" s="66" t="s">
+      <c r="AE2" s="65" t="s">
         <v>447</v>
       </c>
-      <c r="AF2" s="115" t="s">
+      <c r="AF2" s="114" t="s">
         <v>450</v>
       </c>
       <c r="AG2" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="AH2" s="115" t="s">
+      <c r="AH2" s="114" t="s">
         <v>446</v>
       </c>
     </row>
@@ -8246,10 +8080,10 @@
       <c r="A3" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
       <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:34" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8271,16 +8105,16 @@
       <c r="F4" s="29" t="s">
         <v>437</v>
       </c>
-      <c r="G4" s="103" t="s">
+      <c r="G4" s="102" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="83" t="s">
+      <c r="H4" s="82" t="s">
         <v>434</v>
       </c>
-      <c r="I4" s="106" t="s">
+      <c r="I4" s="105" t="s">
         <v>435</v>
       </c>
-      <c r="J4" s="108" t="s">
+      <c r="J4" s="107" t="s">
         <v>438</v>
       </c>
       <c r="K4" s="31" t="s">
@@ -8293,25 +8127,25 @@
       <c r="N4" s="29" t="s">
         <v>440</v>
       </c>
-      <c r="P4" s="109" t="s">
+      <c r="P4" s="108" t="s">
         <v>442</v>
       </c>
-      <c r="Q4" s="110" t="s">
+      <c r="Q4" s="109" t="s">
         <v>445</v>
       </c>
       <c r="R4" s="44" t="s">
         <v>443</v>
       </c>
-      <c r="S4" s="111" t="s">
+      <c r="S4" s="110" t="s">
         <v>444</v>
       </c>
-      <c r="T4" s="88" t="s">
+      <c r="T4" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="U4" s="88" t="s">
+      <c r="U4" s="87" t="s">
         <v>469</v>
       </c>
-      <c r="V4" s="88" t="s">
+      <c r="V4" s="87" t="s">
         <v>472</v>
       </c>
       <c r="W4" t="s">
@@ -8323,31 +8157,31 @@
       <c r="Y4" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="Z4" s="112" t="s">
+      <c r="Z4" s="111" t="s">
         <v>369</v>
       </c>
-      <c r="AA4" s="112">
+      <c r="AA4" s="111">
         <v>289</v>
       </c>
-      <c r="AB4" s="112" t="s">
+      <c r="AB4" s="111" t="s">
         <v>370</v>
       </c>
-      <c r="AC4" s="66" t="s">
+      <c r="AC4" s="65" t="s">
         <v>336</v>
       </c>
       <c r="AD4" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="AE4" s="66" t="s">
+      <c r="AE4" s="65" t="s">
         <v>449</v>
       </c>
-      <c r="AF4" s="115" t="s">
+      <c r="AF4" s="114" t="s">
         <v>451</v>
       </c>
       <c r="AG4" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="AH4" s="115" t="s">
+      <c r="AH4" s="114" t="s">
         <v>453</v>
       </c>
     </row>
@@ -8419,17 +8253,17 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="118" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" style="119" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="117" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" style="118" customWidth="1"/>
     <col min="8" max="10" width="8.7109375" style="9" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" style="3" customWidth="1"/>
     <col min="12" max="13" width="8.7109375" style="2" customWidth="1"/>
     <col min="14" max="16" width="8.7109375" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" style="65"/>
+    <col min="17" max="18" width="9.140625" style="64"/>
     <col min="19" max="20" width="9.140625" style="1"/>
-    <col min="21" max="22" width="9.140625" style="69"/>
+    <col min="21" max="22" width="9.140625" style="68"/>
     <col min="23" max="24" width="9.140625" style="1"/>
-    <col min="25" max="26" width="9.140625" style="131"/>
+    <col min="25" max="26" width="9.140625" style="130"/>
     <col min="27" max="28" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -8446,22 +8280,22 @@
       <c r="D1" s="36" t="s">
         <v>455</v>
       </c>
-      <c r="E1" s="141" t="s">
+      <c r="E1" s="140" t="s">
         <v>476</v>
       </c>
-      <c r="F1" s="135" t="s">
+      <c r="F1" s="134" t="s">
         <v>477</v>
       </c>
-      <c r="G1" s="135" t="s">
+      <c r="G1" s="134" t="s">
         <v>478</v>
       </c>
-      <c r="H1" s="117" t="s">
+      <c r="H1" s="116" t="s">
         <v>456</v>
       </c>
-      <c r="I1" s="117" t="s">
+      <c r="I1" s="116" t="s">
         <v>457</v>
       </c>
-      <c r="J1" s="117" t="s">
+      <c r="J1" s="116" t="s">
         <v>458</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -8482,40 +8316,40 @@
       <c r="P1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="64" t="s">
+      <c r="Q1" s="63" t="s">
         <v>459</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="R1" s="63" t="s">
         <v>460</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="63" t="s">
         <v>459</v>
       </c>
-      <c r="T1" s="64" t="s">
+      <c r="T1" s="63" t="s">
         <v>460</v>
       </c>
-      <c r="U1" s="61" t="s">
+      <c r="U1" s="60" t="s">
         <v>461</v>
       </c>
-      <c r="V1" s="61" t="s">
+      <c r="V1" s="60" t="s">
         <v>462</v>
       </c>
-      <c r="W1" s="61" t="s">
+      <c r="W1" s="60" t="s">
         <v>461</v>
       </c>
-      <c r="X1" s="61" t="s">
+      <c r="X1" s="60" t="s">
         <v>462</v>
       </c>
-      <c r="Y1" s="129" t="s">
+      <c r="Y1" s="128" t="s">
         <v>463</v>
       </c>
-      <c r="Z1" s="129" t="s">
+      <c r="Z1" s="128" t="s">
         <v>464</v>
       </c>
-      <c r="AA1" s="129" t="s">
+      <c r="AA1" s="128" t="s">
         <v>463</v>
       </c>
-      <c r="AB1" s="129" t="s">
+      <c r="AB1" s="128" t="s">
         <v>464</v>
       </c>
     </row>
@@ -8532,25 +8366,25 @@
       <c r="D2" s="29" t="s">
         <v>501</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="121" t="s">
         <v>558</v>
       </c>
-      <c r="F2" s="123" t="s">
+      <c r="F2" s="122" t="s">
         <v>559</v>
       </c>
-      <c r="G2" s="123" t="s">
+      <c r="G2" s="122" t="s">
         <v>560</v>
       </c>
-      <c r="H2" s="124" t="s">
+      <c r="H2" s="123" t="s">
         <v>558</v>
       </c>
-      <c r="I2" s="124" t="s">
+      <c r="I2" s="123" t="s">
         <v>559</v>
       </c>
-      <c r="J2" s="124" t="s">
+      <c r="J2" s="123" t="s">
         <v>560</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="83" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="31" t="s">
@@ -8568,10 +8402,10 @@
       <c r="P2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="66" t="s">
+      <c r="Q2" s="65" t="s">
         <v>497</v>
       </c>
-      <c r="R2" s="127" t="s">
+      <c r="R2" s="126" t="s">
         <v>498</v>
       </c>
       <c r="S2" s="8" t="s">
@@ -8580,10 +8414,10 @@
       <c r="T2" s="15" t="s">
         <v>498</v>
       </c>
-      <c r="U2" s="77" t="s">
+      <c r="U2" s="76" t="s">
         <v>493</v>
       </c>
-      <c r="V2" s="128" t="s">
+      <c r="V2" s="127" t="s">
         <v>494</v>
       </c>
       <c r="W2" s="8" t="s">
@@ -8592,10 +8426,10 @@
       <c r="X2" s="15" t="s">
         <v>494</v>
       </c>
-      <c r="Y2" s="130" t="s">
+      <c r="Y2" s="129" t="s">
         <v>495</v>
       </c>
-      <c r="Z2" s="132" t="s">
+      <c r="Z2" s="131" t="s">
         <v>496</v>
       </c>
       <c r="AA2" s="8" t="s">
@@ -8609,8 +8443,8 @@
       <c r="A3" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="101"/>
-      <c r="K3" s="101"/>
+      <c r="H3" s="100"/>
+      <c r="K3" s="100"/>
       <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:28" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8626,25 +8460,25 @@
       <c r="D4" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="119" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="124" t="s">
         <v>465</v>
       </c>
-      <c r="G4" s="121" t="s">
+      <c r="G4" s="120" t="s">
         <v>465</v>
       </c>
-      <c r="H4" s="83" t="s">
+      <c r="H4" s="82" t="s">
         <v>467</v>
       </c>
-      <c r="I4" s="126" t="s">
+      <c r="I4" s="125" t="s">
         <v>466</v>
       </c>
-      <c r="J4" s="126" t="s">
+      <c r="J4" s="125" t="s">
         <v>466</v>
       </c>
-      <c r="K4" s="84" t="s">
+      <c r="K4" s="83" t="s">
         <v>479</v>
       </c>
       <c r="L4" s="31" t="s">
@@ -8657,10 +8491,10 @@
       <c r="O4" s="29" t="s">
         <v>482</v>
       </c>
-      <c r="Q4" s="66" t="s">
+      <c r="Q4" s="65" t="s">
         <v>484</v>
       </c>
-      <c r="R4" s="66" t="s">
+      <c r="R4" s="65" t="s">
         <v>483</v>
       </c>
       <c r="S4" s="8" t="s">
@@ -8669,10 +8503,10 @@
       <c r="T4" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="U4" s="77" t="s">
+      <c r="U4" s="76" t="s">
         <v>487</v>
       </c>
-      <c r="V4" s="77" t="s">
+      <c r="V4" s="76" t="s">
         <v>488</v>
       </c>
       <c r="W4" s="8" t="s">
@@ -8681,10 +8515,10 @@
       <c r="X4" s="8" t="s">
         <v>490</v>
       </c>
-      <c r="Y4" s="130" t="s">
+      <c r="Y4" s="129" t="s">
         <v>491</v>
       </c>
-      <c r="Z4" s="130" t="s">
+      <c r="Z4" s="129" t="s">
         <v>490</v>
       </c>
       <c r="AA4" s="8" t="s">
@@ -8749,11 +8583,11 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="118" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="119" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="119" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="119" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="119" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="117" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="118" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="118" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="118" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="118" customWidth="1"/>
     <col min="10" max="11" width="8.7109375" style="9" customWidth="1"/>
     <col min="12" max="12" width="17.85546875" style="9" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" style="9" customWidth="1"/>
@@ -8761,8 +8595,8 @@
     <col min="15" max="15" width="8.7109375" style="3" customWidth="1"/>
     <col min="16" max="17" width="8.7109375" style="2" customWidth="1"/>
     <col min="18" max="20" width="8.7109375" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" style="65" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" style="64" customWidth="1"/>
     <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8" customWidth="1"/>
   </cols>
@@ -8780,34 +8614,34 @@
       <c r="D1" t="s">
         <v>503</v>
       </c>
-      <c r="E1" s="141" t="s">
+      <c r="E1" s="140" t="s">
         <v>476</v>
       </c>
-      <c r="F1" s="142" t="s">
+      <c r="F1" s="141" t="s">
         <v>523</v>
       </c>
-      <c r="G1" s="135" t="s">
+      <c r="G1" s="134" t="s">
         <v>505</v>
       </c>
-      <c r="H1" s="142" t="s">
+      <c r="H1" s="141" t="s">
         <v>506</v>
       </c>
-      <c r="I1" s="135" t="s">
+      <c r="I1" s="134" t="s">
         <v>507</v>
       </c>
-      <c r="J1" s="135" t="s">
+      <c r="J1" s="134" t="s">
         <v>476</v>
       </c>
-      <c r="K1" s="142" t="s">
+      <c r="K1" s="141" t="s">
         <v>523</v>
       </c>
-      <c r="L1" s="135" t="s">
+      <c r="L1" s="134" t="s">
         <v>505</v>
       </c>
-      <c r="M1" s="142" t="s">
+      <c r="M1" s="141" t="s">
         <v>506</v>
       </c>
-      <c r="N1" s="135" t="s">
+      <c r="N1" s="134" t="s">
         <v>507</v>
       </c>
       <c r="O1" s="5" t="s">
@@ -8828,63 +8662,63 @@
       <c r="T1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="V1" s="64" t="s">
+      <c r="V1" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="W1" s="64" t="s">
+      <c r="W1" s="63" t="s">
         <v>352</v>
       </c>
-      <c r="X1" s="64" t="s">
+      <c r="X1" s="63" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="132" t="s">
         <v>521</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="133" t="s">
+      <c r="C2" s="132" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="133" t="s">
+      <c r="D2" s="132" t="s">
         <v>504</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="121" t="s">
         <v>514</v>
       </c>
-      <c r="F2" s="123" t="s">
+      <c r="F2" s="122" t="s">
         <v>515</v>
       </c>
-      <c r="G2" s="123" t="s">
+      <c r="G2" s="122" t="s">
         <v>509</v>
       </c>
-      <c r="H2" s="123" t="s">
+      <c r="H2" s="122" t="s">
         <v>508</v>
       </c>
-      <c r="I2" s="123" t="s">
+      <c r="I2" s="122" t="s">
         <v>516</v>
       </c>
-      <c r="J2" s="124" t="s">
+      <c r="J2" s="123" t="s">
         <v>514</v>
       </c>
-      <c r="K2" s="124" t="s">
+      <c r="K2" s="123" t="s">
         <v>515</v>
       </c>
-      <c r="L2" s="124" t="s">
+      <c r="L2" s="123" t="s">
         <v>509</v>
       </c>
-      <c r="M2" s="124" t="s">
+      <c r="M2" s="123" t="s">
         <v>508</v>
       </c>
-      <c r="N2" s="124" t="s">
+      <c r="N2" s="123" t="s">
         <v>516</v>
       </c>
-      <c r="O2" s="84" t="s">
+      <c r="O2" s="83" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="31" t="s">
@@ -8902,10 +8736,10 @@
       <c r="T2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="66" t="s">
+      <c r="U2" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="V2" s="66" t="s">
+      <c r="V2" s="65" t="s">
         <v>361</v>
       </c>
       <c r="W2" s="29" t="s">
@@ -8919,11 +8753,11 @@
       <c r="A3" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="134"/>
-      <c r="H3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="O3" s="101"/>
+      <c r="E3" s="133"/>
+      <c r="H3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="O3" s="100"/>
       <c r="R3" s="28"/>
     </row>
     <row r="4" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8939,35 +8773,35 @@
       <c r="D4" s="29" t="s">
         <v>522</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="119" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="124" t="s">
         <v>465</v>
       </c>
-      <c r="G4" s="136" t="s">
+      <c r="G4" s="135" t="s">
         <v>510</v>
       </c>
-      <c r="H4" s="121" t="s">
+      <c r="H4" s="120" t="s">
         <v>511</v>
       </c>
-      <c r="I4" s="138" t="s">
+      <c r="I4" s="137" t="s">
         <v>512</v>
       </c>
-      <c r="J4" s="83" t="s">
+      <c r="J4" s="82" t="s">
         <v>467</v>
       </c>
-      <c r="K4" s="126" t="s">
+      <c r="K4" s="125" t="s">
         <v>466</v>
       </c>
-      <c r="L4" s="139" t="s">
+      <c r="L4" s="138" t="s">
         <v>513</v>
       </c>
-      <c r="M4" s="83" t="s">
+      <c r="M4" s="82" t="s">
         <v>511</v>
       </c>
-      <c r="N4" s="137"/>
-      <c r="O4" s="84" t="s">
+      <c r="N4" s="136"/>
+      <c r="O4" s="83" t="s">
         <v>479</v>
       </c>
       <c r="P4" s="31" t="s">
@@ -8980,16 +8814,16 @@
       <c r="S4" s="29" t="s">
         <v>482</v>
       </c>
-      <c r="U4" s="109" t="s">
+      <c r="U4" s="108" t="s">
         <v>517</v>
       </c>
-      <c r="V4" s="140" t="s">
+      <c r="V4" s="139" t="s">
         <v>518</v>
       </c>
       <c r="W4" s="44" t="s">
         <v>519</v>
       </c>
-      <c r="X4" s="111" t="s">
+      <c r="X4" s="110" t="s">
         <v>444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EE-1870 - Added the template change to the commit Mistakenly didn't add the template change to the last commit.
</commit_message>
<xml_diff>
--- a/templates/sequence-based-metadata/EGA_metadata_submission_template_v1.xlsx
+++ b/templates/sequence-based-metadata/EGA_metadata_submission_template_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcasado\Documents\GitHub\ega-metadata-schema\templates\sequence-based-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8B9E9B-4DDA-454D-94D0-8D841627A2F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E424FC-763B-4C4D-8BEB-CC943D8F5AAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="566">
   <si>
     <t>Tag</t>
   </si>
@@ -2468,6 +2468,15 @@
   </si>
   <si>
     <t>TODO: More extensive free-form description of the Dataset.  It should include the content of the dataset (number of samples, file types, technology/protocol used to obtain the data…) and not contain more than 4 sentences.</t>
+  </si>
+  <si>
+    <t>TODO: leave this column empty, for subject_id will contain no units.</t>
+  </si>
+  <si>
+    <t>TODO: leave this column empty, for sex will contain no units.</t>
+  </si>
+  <si>
+    <t>TODO: leave this column empty, for phenotype will contain no units.</t>
   </si>
 </sst>
 </file>
@@ -5439,13 +5448,13 @@
     <col min="8" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="7.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="6.42578125" style="25" customWidth="1"/>
     <col min="19" max="19" width="6.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.28515625" style="2" customWidth="1"/>
@@ -5620,21 +5629,27 @@
       <c r="J2" s="31" t="s">
         <v>552</v>
       </c>
-      <c r="K2" s="31"/>
+      <c r="K2" s="31" t="s">
+        <v>563</v>
+      </c>
       <c r="L2" s="8" t="s">
         <v>291</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>553</v>
       </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="8" t="s">
+        <v>564</v>
+      </c>
       <c r="O2" s="31" t="s">
         <v>292</v>
       </c>
       <c r="P2" s="31" t="s">
         <v>554</v>
       </c>
-      <c r="Q2" s="31"/>
+      <c r="Q2" s="31" t="s">
+        <v>565</v>
+      </c>
       <c r="R2" s="30" t="s">
         <v>293</v>
       </c>

</xml_diff>